<commit_message>
DD and DT updates
</commit_message>
<xml_diff>
--- a/input/l2/WHO-SRH-21.2-eng.xlsx
+++ b/input/l2/WHO-SRH-21.2-eng.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Adam/Src/who-int/anc-cds/input/l2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372D6153-77BC-6449-BD77-3432E36CD55F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF61CE34-1BB5-B542-984D-B5E9E10DE8EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11260" yWindow="1060" windowWidth="26060" windowHeight="17620" firstSheet="6" activeTab="9" xr2:uid="{8743308B-CEBB-4E83-A8A2-EC270BF9A959}"/>
+    <workbookView xWindow="600" yWindow="1500" windowWidth="26060" windowHeight="17620" firstSheet="11" activeTab="16" xr2:uid="{8743308B-CEBB-4E83-A8A2-EC270BF9A959}"/>
   </bookViews>
   <sheets>
     <sheet name="FP.LO.004-3. PregTestNegative" sheetId="26" state="hidden" r:id="rId1"/>
@@ -10860,7 +10860,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="636">
+  <cellXfs count="637">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -12772,6 +12772,9 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -14113,7 +14116,7 @@
   </sheetPr>
   <dimension ref="A2:EK75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -19418,8 +19421,8 @@
   </sheetPr>
   <dimension ref="A2:J105"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D99" sqref="D99"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25339,8 +25342,8 @@
   </sheetPr>
   <dimension ref="A2:HA21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29532,8 +29535,8 @@
   </sheetPr>
   <dimension ref="B1:K47"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30179,7 +30182,7 @@
       <c r="C36" s="300" t="s">
         <v>1010</v>
       </c>
-      <c r="D36" s="600" t="s">
+      <c r="D36" s="636" t="s">
         <v>1011</v>
       </c>
       <c r="E36" s="600"/>
@@ -30342,7 +30345,7 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="D40" workbookViewId="0">
       <selection activeCell="C10" sqref="C10:E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>